<commit_message>
Long day of work
</commit_message>
<xml_diff>
--- a/Tables/Table 3 - ZmIonome Candidate Genes.xlsx
+++ b/Tables/Table 3 - ZmIonome Candidate Genes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="58">
   <si>
     <t>500kb</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>500KB</t>
+  </si>
+  <si>
+    <t>Ionome (Average)</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -777,6 +780,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -801,59 +858,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1137,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="A22" sqref="A22:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,22 +1189,22 @@
       <c r="B1" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33" t="s">
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1189,21 +1222,21 @@
       <c r="E2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33" t="s">
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1253,122 +1286,122 @@
       <c r="A4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="33">
         <v>4243</v>
       </c>
-      <c r="C4" s="42">
+      <c r="C4" s="34">
         <v>2279</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="34">
         <v>1658</v>
       </c>
-      <c r="E4" s="42">
+      <c r="E4" s="34">
         <v>456</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="34">
         <v>5272</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="34">
         <v>7348</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="34">
         <v>11612</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="34">
         <v>7727</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="34">
         <v>9664</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="34">
         <v>13614</v>
       </c>
-      <c r="L4" s="42">
+      <c r="L4" s="34">
         <v>20024</v>
       </c>
-      <c r="M4" s="42">
+      <c r="M4" s="34">
         <v>20776</v>
       </c>
-      <c r="N4" s="43">
+      <c r="N4" s="35">
         <v>22927</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="56">
+      <c r="B5" s="48">
         <v>176</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="36">
         <v>149</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="37">
         <v>140</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="38">
         <v>98</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="36">
         <v>239</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="37">
         <v>336</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="43">
         <v>417</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="45">
         <v>350</v>
       </c>
-      <c r="J5" s="45">
+      <c r="J5" s="37">
         <v>523</v>
       </c>
-      <c r="K5" s="51">
+      <c r="K5" s="43">
         <v>699</v>
       </c>
-      <c r="L5" s="45">
+      <c r="L5" s="37">
         <v>804</v>
       </c>
-      <c r="M5" s="45">
+      <c r="M5" s="37">
         <v>1035</v>
       </c>
-      <c r="N5" s="46">
+      <c r="N5" s="38">
         <v>1684</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="57">
+      <c r="B6" s="49">
         <v>182</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="39">
         <v>151</v>
       </c>
       <c r="D6" s="32">
         <v>141</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="40">
         <v>104</v>
       </c>
-      <c r="F6" s="47">
+      <c r="F6" s="39">
         <v>228</v>
       </c>
       <c r="G6" s="32">
         <v>314</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="44">
         <v>372</v>
       </c>
-      <c r="I6" s="54">
+      <c r="I6" s="46">
         <v>339</v>
       </c>
       <c r="J6" s="32">
         <v>489</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="44">
         <v>669</v>
       </c>
       <c r="L6" s="32">
@@ -1377,42 +1410,42 @@
       <c r="M6" s="32">
         <v>986</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="40">
         <v>1657</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="57">
+      <c r="B7" s="49">
         <v>108</v>
       </c>
-      <c r="C7" s="47">
+      <c r="C7" s="39">
         <v>95</v>
       </c>
       <c r="D7" s="32">
         <v>86</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="40">
         <v>68</v>
       </c>
-      <c r="F7" s="47">
+      <c r="F7" s="39">
         <v>154</v>
       </c>
       <c r="G7" s="32">
         <v>233</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="44">
         <v>271</v>
       </c>
-      <c r="I7" s="54">
+      <c r="I7" s="46">
         <v>219</v>
       </c>
       <c r="J7" s="32">
         <v>326</v>
       </c>
-      <c r="K7" s="52">
+      <c r="K7" s="44">
         <v>433</v>
       </c>
       <c r="L7" s="32">
@@ -1421,42 +1454,42 @@
       <c r="M7" s="32">
         <v>601</v>
       </c>
-      <c r="N7" s="48">
+      <c r="N7" s="40">
         <v>1007</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="57">
+      <c r="B8" s="49">
         <v>105</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="39">
         <v>82</v>
       </c>
       <c r="D8" s="32">
         <v>78</v>
       </c>
-      <c r="E8" s="48">
+      <c r="E8" s="40">
         <v>61</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="39">
         <v>124</v>
       </c>
       <c r="G8" s="32">
         <v>181</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="44">
         <v>215</v>
       </c>
-      <c r="I8" s="54">
+      <c r="I8" s="46">
         <v>164</v>
       </c>
       <c r="J8" s="32">
         <v>253</v>
       </c>
-      <c r="K8" s="52">
+      <c r="K8" s="44">
         <v>350</v>
       </c>
       <c r="L8" s="32">
@@ -1465,42 +1498,42 @@
       <c r="M8" s="32">
         <v>476</v>
       </c>
-      <c r="N8" s="48">
+      <c r="N8" s="40">
         <v>845</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="57">
+      <c r="B9" s="49">
         <v>630</v>
       </c>
-      <c r="C9" s="47">
+      <c r="C9" s="39">
         <v>471</v>
       </c>
       <c r="D9" s="32">
         <v>418</v>
       </c>
-      <c r="E9" s="48">
+      <c r="E9" s="40">
         <v>251</v>
       </c>
-      <c r="F9" s="47">
+      <c r="F9" s="39">
         <v>869</v>
       </c>
       <c r="G9" s="32">
         <v>1189</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="44">
         <v>1395</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="46">
         <v>1252</v>
       </c>
       <c r="J9" s="32">
         <v>1786</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="44">
         <v>2309</v>
       </c>
       <c r="L9" s="32">
@@ -1509,42 +1542,42 @@
       <c r="M9" s="32">
         <v>3758</v>
       </c>
-      <c r="N9" s="48">
+      <c r="N9" s="40">
         <v>5283</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="57">
+      <c r="B10" s="49">
         <v>165</v>
       </c>
-      <c r="C10" s="47">
+      <c r="C10" s="39">
         <v>133</v>
       </c>
       <c r="D10" s="32">
         <v>125</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="40">
         <v>101</v>
       </c>
-      <c r="F10" s="47">
+      <c r="F10" s="39">
         <v>202</v>
       </c>
       <c r="G10" s="32">
         <v>293</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="44">
         <v>355</v>
       </c>
-      <c r="I10" s="54">
+      <c r="I10" s="46">
         <v>284</v>
       </c>
       <c r="J10" s="32">
         <v>437</v>
       </c>
-      <c r="K10" s="52">
+      <c r="K10" s="44">
         <v>604</v>
       </c>
       <c r="L10" s="32">
@@ -1553,42 +1586,42 @@
       <c r="M10" s="32">
         <v>805</v>
       </c>
-      <c r="N10" s="48">
+      <c r="N10" s="40">
         <v>1431</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="57">
+      <c r="B11" s="49">
         <v>171</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="39">
         <v>136</v>
       </c>
       <c r="D11" s="32">
         <v>125</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="40">
         <v>89</v>
       </c>
-      <c r="F11" s="47">
+      <c r="F11" s="39">
         <v>252</v>
       </c>
       <c r="G11" s="32">
         <v>351</v>
       </c>
-      <c r="H11" s="52">
+      <c r="H11" s="44">
         <v>420</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="46">
         <v>335</v>
       </c>
       <c r="J11" s="32">
         <v>511</v>
       </c>
-      <c r="K11" s="52">
+      <c r="K11" s="44">
         <v>697</v>
       </c>
       <c r="L11" s="32">
@@ -1597,42 +1630,42 @@
       <c r="M11" s="32">
         <v>990</v>
       </c>
-      <c r="N11" s="48">
+      <c r="N11" s="40">
         <v>1546</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="57">
+      <c r="B12" s="49">
         <v>130</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="39">
         <v>111</v>
       </c>
       <c r="D12" s="32">
         <v>100</v>
       </c>
-      <c r="E12" s="48">
+      <c r="E12" s="40">
         <v>78</v>
       </c>
-      <c r="F12" s="47">
+      <c r="F12" s="39">
         <v>168</v>
       </c>
       <c r="G12" s="32">
         <v>248</v>
       </c>
-      <c r="H12" s="52">
+      <c r="H12" s="44">
         <v>298</v>
       </c>
-      <c r="I12" s="54">
+      <c r="I12" s="46">
         <v>239</v>
       </c>
       <c r="J12" s="32">
         <v>357</v>
       </c>
-      <c r="K12" s="52">
+      <c r="K12" s="44">
         <v>498</v>
       </c>
       <c r="L12" s="32">
@@ -1641,42 +1674,42 @@
       <c r="M12" s="32">
         <v>715</v>
       </c>
-      <c r="N12" s="48">
+      <c r="N12" s="40">
         <v>1176</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="57">
+      <c r="B13" s="49">
         <v>153</v>
       </c>
-      <c r="C13" s="47">
+      <c r="C13" s="39">
         <v>129</v>
       </c>
       <c r="D13" s="32">
         <v>121</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="40">
         <v>99</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="39">
         <v>203</v>
       </c>
       <c r="G13" s="32">
         <v>281</v>
       </c>
-      <c r="H13" s="52">
+      <c r="H13" s="44">
         <v>328</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="46">
         <v>274</v>
       </c>
       <c r="J13" s="32">
         <v>414</v>
       </c>
-      <c r="K13" s="52">
+      <c r="K13" s="44">
         <v>554</v>
       </c>
       <c r="L13" s="32">
@@ -1685,42 +1718,42 @@
       <c r="M13" s="32">
         <v>815</v>
       </c>
-      <c r="N13" s="48">
+      <c r="N13" s="40">
         <v>1398</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="57">
+      <c r="B14" s="49">
         <v>168</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="39">
         <v>134</v>
       </c>
       <c r="D14" s="32">
         <v>119</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="40">
         <v>94</v>
       </c>
-      <c r="F14" s="47">
+      <c r="F14" s="39">
         <v>228</v>
       </c>
       <c r="G14" s="32">
         <v>302</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="44">
         <v>340</v>
       </c>
-      <c r="I14" s="54">
+      <c r="I14" s="46">
         <v>314</v>
       </c>
       <c r="J14" s="32">
         <v>436</v>
       </c>
-      <c r="K14" s="52">
+      <c r="K14" s="44">
         <v>562</v>
       </c>
       <c r="L14" s="32">
@@ -1729,42 +1762,42 @@
       <c r="M14" s="32">
         <v>850</v>
       </c>
-      <c r="N14" s="48">
+      <c r="N14" s="40">
         <v>1364</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="57">
+      <c r="B15" s="49">
         <v>154</v>
       </c>
-      <c r="C15" s="47">
+      <c r="C15" s="39">
         <v>123</v>
       </c>
       <c r="D15" s="32">
         <v>109</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="40">
         <v>74</v>
       </c>
-      <c r="F15" s="47">
+      <c r="F15" s="39">
         <v>226</v>
       </c>
       <c r="G15" s="32">
         <v>312</v>
       </c>
-      <c r="H15" s="52">
+      <c r="H15" s="44">
         <v>361</v>
       </c>
-      <c r="I15" s="54">
+      <c r="I15" s="46">
         <v>287</v>
       </c>
       <c r="J15" s="32">
         <v>419</v>
       </c>
-      <c r="K15" s="52">
+      <c r="K15" s="44">
         <v>532</v>
       </c>
       <c r="L15" s="32">
@@ -1773,42 +1806,42 @@
       <c r="M15" s="32">
         <v>892</v>
       </c>
-      <c r="N15" s="48">
+      <c r="N15" s="40">
         <v>1354</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="49">
         <v>99</v>
       </c>
-      <c r="C16" s="47">
+      <c r="C16" s="39">
         <v>73</v>
       </c>
       <c r="D16" s="32">
         <v>64</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="40">
         <v>49</v>
       </c>
-      <c r="F16" s="47">
+      <c r="F16" s="39">
         <v>107</v>
       </c>
       <c r="G16" s="32">
         <v>148</v>
       </c>
-      <c r="H16" s="52">
+      <c r="H16" s="44">
         <v>163</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="46">
         <v>161</v>
       </c>
       <c r="J16" s="32">
         <v>226</v>
       </c>
-      <c r="K16" s="52">
+      <c r="K16" s="44">
         <v>291</v>
       </c>
       <c r="L16" s="32">
@@ -1817,42 +1850,42 @@
       <c r="M16" s="32">
         <v>417</v>
       </c>
-      <c r="N16" s="48">
+      <c r="N16" s="40">
         <v>697</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="57">
+      <c r="B17" s="49">
         <v>123</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="39">
         <v>101</v>
       </c>
       <c r="D17" s="32">
         <v>91</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="40">
         <v>70</v>
       </c>
-      <c r="F17" s="47">
+      <c r="F17" s="39">
         <v>159</v>
       </c>
       <c r="G17" s="32">
         <v>223</v>
       </c>
-      <c r="H17" s="52">
+      <c r="H17" s="44">
         <v>260</v>
       </c>
-      <c r="I17" s="54">
+      <c r="I17" s="46">
         <v>210</v>
       </c>
       <c r="J17" s="32">
         <v>312</v>
       </c>
-      <c r="K17" s="52">
+      <c r="K17" s="44">
         <v>424</v>
       </c>
       <c r="L17" s="32">
@@ -1861,42 +1894,42 @@
       <c r="M17" s="32">
         <v>643</v>
       </c>
-      <c r="N17" s="48">
+      <c r="N17" s="40">
         <v>1051</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="57">
+      <c r="B18" s="49">
         <v>135</v>
       </c>
-      <c r="C18" s="47">
+      <c r="C18" s="39">
         <v>105</v>
       </c>
       <c r="D18" s="32">
         <v>93</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="40">
         <v>78</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="39">
         <v>168</v>
       </c>
       <c r="G18" s="32">
         <v>223</v>
       </c>
-      <c r="H18" s="52">
+      <c r="H18" s="44">
         <v>251</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="46">
         <v>245</v>
       </c>
       <c r="J18" s="32">
         <v>335</v>
       </c>
-      <c r="K18" s="52">
+      <c r="K18" s="44">
         <v>414</v>
       </c>
       <c r="L18" s="32">
@@ -1905,42 +1938,42 @@
       <c r="M18" s="32">
         <v>590</v>
       </c>
-      <c r="N18" s="48">
+      <c r="N18" s="40">
         <v>1026</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="57">
+      <c r="B19" s="49">
         <v>162</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="39">
         <v>135</v>
       </c>
       <c r="D19" s="32">
         <v>129</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="40">
         <v>101</v>
       </c>
-      <c r="F19" s="47">
+      <c r="F19" s="39">
         <v>237</v>
       </c>
       <c r="G19" s="32">
         <v>328</v>
       </c>
-      <c r="H19" s="52">
+      <c r="H19" s="44">
         <v>392</v>
       </c>
-      <c r="I19" s="54">
+      <c r="I19" s="46">
         <v>330</v>
       </c>
       <c r="J19" s="32">
         <v>485</v>
       </c>
-      <c r="K19" s="52">
+      <c r="K19" s="44">
         <v>682</v>
       </c>
       <c r="L19" s="32">
@@ -1949,42 +1982,42 @@
       <c r="M19" s="32">
         <v>895</v>
       </c>
-      <c r="N19" s="48">
+      <c r="N19" s="40">
         <v>1563</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="57">
+      <c r="B20" s="49">
         <v>113</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="39">
         <v>99</v>
       </c>
       <c r="D20" s="32">
         <v>90</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="40">
         <v>63</v>
       </c>
-      <c r="F20" s="47">
+      <c r="F20" s="39">
         <v>142</v>
       </c>
       <c r="G20" s="32">
         <v>206</v>
       </c>
-      <c r="H20" s="52">
+      <c r="H20" s="44">
         <v>238</v>
       </c>
-      <c r="I20" s="54">
+      <c r="I20" s="46">
         <v>199</v>
       </c>
       <c r="J20" s="32">
         <v>317</v>
       </c>
-      <c r="K20" s="52">
+      <c r="K20" s="44">
         <v>431</v>
       </c>
       <c r="L20" s="32">
@@ -1993,27 +2026,27 @@
       <c r="M20" s="32">
         <v>636</v>
       </c>
-      <c r="N20" s="48">
+      <c r="N20" s="40">
         <v>1009</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="58">
+      <c r="B21" s="50">
         <v>149</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="41">
         <v>125</v>
       </c>
       <c r="D21" s="8">
         <v>116</v>
       </c>
-      <c r="E21" s="50">
+      <c r="E21" s="42">
         <v>90</v>
       </c>
-      <c r="F21" s="49">
+      <c r="F21" s="41">
         <v>211</v>
       </c>
       <c r="G21" s="8">
@@ -2022,7 +2055,7 @@
       <c r="H21" s="9">
         <v>348</v>
       </c>
-      <c r="I21" s="55">
+      <c r="I21" s="47">
         <v>288</v>
       </c>
       <c r="J21" s="8">
@@ -2037,12 +2070,95 @@
       <c r="M21" s="8">
         <v>841</v>
       </c>
-      <c r="N21" s="50">
+      <c r="N21" s="42">
         <v>1419</v>
       </c>
     </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="67">
+        <f>AVERAGE(B5:B21)</f>
+        <v>171.94117647058823</v>
+      </c>
+      <c r="C22" s="65">
+        <f>AVERAGE(C5:C21)</f>
+        <v>138.35294117647058</v>
+      </c>
+      <c r="D22" s="60">
+        <f t="shared" ref="D22:E22" si="0">AVERAGE(D5:D21)</f>
+        <v>126.17647058823529</v>
+      </c>
+      <c r="E22" s="61">
+        <f t="shared" si="0"/>
+        <v>92.235294117647058</v>
+      </c>
+      <c r="F22" s="60">
+        <f t="shared" ref="F22" si="1">AVERAGE(F5:F21)</f>
+        <v>230.41176470588235</v>
+      </c>
+      <c r="G22" s="60">
+        <f t="shared" ref="G22" si="2">AVERAGE(G5:G21)</f>
+        <v>321.58823529411762</v>
+      </c>
+      <c r="H22" s="60">
+        <f t="shared" ref="H22" si="3">AVERAGE(H5:H21)</f>
+        <v>377.88235294117646</v>
+      </c>
+      <c r="I22" s="60">
+        <f t="shared" ref="I22" si="4">AVERAGE(I5:I21)</f>
+        <v>322.94117647058823</v>
+      </c>
+      <c r="J22" s="60">
+        <f t="shared" ref="J22" si="5">AVERAGE(J5:J21)</f>
+        <v>474.1764705882353</v>
+      </c>
+      <c r="K22" s="60">
+        <f t="shared" ref="K22" si="6">AVERAGE(K5:K21)</f>
+        <v>630.23529411764707</v>
+      </c>
+      <c r="L22" s="60">
+        <f t="shared" ref="L22" si="7">AVERAGE(L5:L21)</f>
+        <v>718.41176470588232</v>
+      </c>
+      <c r="M22" s="60">
+        <f t="shared" ref="M22" si="8">AVERAGE(M5:M21)</f>
+        <v>937.94117647058829</v>
+      </c>
+      <c r="N22" s="61">
+        <f t="shared" ref="N22" si="9">AVERAGE(N5:N21)</f>
+        <v>1500.5882352941176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="62"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="66">
+        <f>AVERAGE(C22:E22)</f>
+        <v>118.92156862745098</v>
+      </c>
+      <c r="D23" s="63"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="63">
+        <f>AVERAGE(F22:N22)</f>
+        <v>612.68627450980387</v>
+      </c>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="64"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="F23:N23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:N2"/>
@@ -2100,22 +2216,22 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -2125,22 +2241,22 @@
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="36"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="54"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
@@ -2165,21 +2281,21 @@
       <c r="F3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35" t="s">
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35" t="s">
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="36"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54"/>
     </row>
     <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
@@ -3174,16 +3290,16 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-      <c r="K42" s="34"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>